<commit_message>
update finance template: shorthand -> shorthand fee
</commit_message>
<xml_diff>
--- a/public/templates/finance_template.xlsx
+++ b/public/templates/finance_template.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'2019.12'!$A$1:$AK$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'2019.12'!$A$1:$AK$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'2019.12'!$A$1:$AK$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'2019.12'!$A$1:$AK$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -73,7 +74,7 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Shorthand</t>
+    <t>Shorthand Fee</t>
   </si>
   <si>
     <r>
@@ -195,7 +196,7 @@
     <t>备注</t>
   </si>
   <si>
-    <t>速记</t>
+    <t>速记费</t>
   </si>
   <si>
     <r>
@@ -506,8 +507,8 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -547,7 +548,7 @@
     <col collapsed="false" hidden="false" max="1025" min="34" style="1" width="8.66396761133603"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>